<commit_message>
Added GM selection for steelSDA
</commit_message>
<xml_diff>
--- a/Modules/RCWallSDA/Input.xlsx
+++ b/Modules/RCWallSDA/Input.xlsx
@@ -610,7 +610,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -634,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>1.3</v>

</xml_diff>